<commit_message>
Fix the N2 levels and update notebook "N2 double pulse simulation (79.4 fs, 1T).ipynb"
</commit_message>
<xml_diff>
--- a/Notebooks/simul/rsc/n2_levels.xlsx
+++ b/Notebooks/simul/rsc/n2_levels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Dropbox/FERMI 20149100 Ueda/Notebooks/simul/rsc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5218390E-99BC-084E-93AE-D6B5C3098945}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26663DCE-3587-CC4B-A25B-32D1DD7BED1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40240" yWindow="460" windowWidth="33600" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47060" yWindow="-680" windowWidth="33600" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Levels" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,14 @@
     <sheet name="Ionization" sheetId="3" r:id="rId3"/>
     <sheet name="References" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -690,11 +697,11 @@
   </sheetPr>
   <dimension ref="A1:K956"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:K1048576"/>
+      <selection pane="bottomRight" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2485,7 +2492,7 @@
         <v>7.9857293746699645</v>
       </c>
       <c r="I48" s="6">
-        <v>1.64</v>
+        <v>0</v>
       </c>
       <c r="J48" s="13"/>
       <c r="K48" s="2">
@@ -2584,7 +2591,7 @@
         <v>8.0881407444606452</v>
       </c>
       <c r="I51" s="6">
-        <v>0</v>
+        <v>1.64</v>
       </c>
       <c r="J51" s="13"/>
       <c r="K51" s="2">
@@ -16785,7 +16792,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>